<commit_message>
implement outputJson option and verbose option.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestTask.xlsx
+++ b/meta/program/BlancoRestAutotestTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD46A73-3295-2544-B2AA-50E0B9B57C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADA17D1-BE2A-6246-89BA-840E55A2121A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15740" yWindow="1120" windowWidth="22660" windowHeight="15620" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -276,6 +276,20 @@
   </si>
   <si>
     <t>BlancoRestAutotestのAntTaskです。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>outputJson</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>電文をJSONファイルとして出力します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">シュツリョク </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -748,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -865,6 +879,24 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -884,24 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1338,10 +1353,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1387,10 +1402,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="68"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="6" t="s">
         <v>48</v>
       </c>
@@ -1400,10 +1415,10 @@
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="68"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="58" t="s">
         <v>49</v>
       </c>
@@ -1414,10 +1429,10 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="68"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="6" t="s">
         <v>50</v>
       </c>
@@ -1428,10 +1443,10 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="68"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
@@ -1463,38 +1478,38 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="69" t="s">
+      <c r="F12" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="71"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="44">
@@ -1531,12 +1546,12 @@
       <c r="E15" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="77"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="70"/>
     </row>
     <row r="16" spans="1:9" ht="26.25" customHeight="1">
       <c r="A16" s="51">
@@ -1552,12 +1567,12 @@
       <c r="E16" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="75" t="s">
+      <c r="F16" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="77"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
     </row>
     <row r="17" spans="1:9" ht="26.25" customHeight="1">
       <c r="A17" s="51">
@@ -1571,12 +1586,12 @@
       </c>
       <c r="D17" s="54"/>
       <c r="E17" s="52"/>
-      <c r="F17" s="78" t="s">
+      <c r="F17" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="79"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="80"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="73"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="22">
@@ -1663,26 +1678,47 @@
       <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="42"/>
+      <c r="A22" s="22">
+        <v>7</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>22</v>
+      </c>
       <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
+      <c r="E22" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="81" t="s">
+        <v>52</v>
+      </c>
       <c r="G22" s="26"/>
       <c r="H22" s="26"/>
       <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="33"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1702,14 +1738,14 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F40" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>